<commit_message>
Added 13 new units
</commit_message>
<xml_diff>
--- a/documentation/allStats.xlsx
+++ b/documentation/allStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\project_aeii\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C93BB3-0B47-4DD9-8E12-54601FB0879C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF273B8-3CC1-42CE-969F-9179FB21D7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7650" yWindow="7440" windowWidth="15345" windowHeight="10035" xr2:uid="{D4135FBB-2C8A-48D4-BC1E-A4B2555D16E4}"/>
+    <workbookView xWindow="20895" yWindow="3555" windowWidth="15345" windowHeight="10035" xr2:uid="{D4135FBB-2C8A-48D4-BC1E-A4B2555D16E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Dataset</t>
   </si>
@@ -177,15 +177,9 @@
     <t>5, 11, 26</t>
   </si>
   <si>
-    <t>Black Mages</t>
-  </si>
-  <si>
     <t>Wolf</t>
   </si>
   <si>
-    <t>8, 16, 26</t>
-  </si>
-  <si>
     <t>Blop</t>
   </si>
   <si>
@@ -196,6 +190,69 @@
   </si>
   <si>
     <t>27, 28</t>
+  </si>
+  <si>
+    <t>Civilian</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Mace bearer</t>
+  </si>
+  <si>
+    <t>Lancer</t>
+  </si>
+  <si>
+    <t>17, 20, 25</t>
+  </si>
+  <si>
+    <t>Armored Lancer</t>
+  </si>
+  <si>
+    <t>17, 20, 25, 28</t>
+  </si>
+  <si>
+    <t>Orball Witch</t>
+  </si>
+  <si>
+    <t>Black Mage</t>
+  </si>
+  <si>
+    <t>Orball Warrior</t>
+  </si>
+  <si>
+    <t>0, 8, 24</t>
+  </si>
+  <si>
+    <t>Iron Golem</t>
+  </si>
+  <si>
+    <t>4, 17</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Skeleton Warrior</t>
+  </si>
+  <si>
+    <t>Skeleton Mage</t>
+  </si>
+  <si>
+    <t>Demon</t>
+  </si>
+  <si>
+    <t>2, 4, 11, 14, 17, 25</t>
+  </si>
+  <si>
+    <t>Viking</t>
+  </si>
+  <si>
+    <t>0, 1, 2, 8, 13, 14, 20</t>
+  </si>
+  <si>
+    <t>8, 16, 26, 2, 14</t>
   </si>
 </sst>
 </file>
@@ -555,14 +612,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE6564-BC17-41CE-A57A-346809BD4733}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="17" width="13.140625" customWidth="1"/>
+    <col min="2" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="17" width="13.140625" customWidth="1"/>
     <col min="18" max="18" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1007,7 +1066,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1016,7 +1075,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>19</v>
@@ -1382,7 +1441,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1">
         <v>600</v>
@@ -1434,7 +1493,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1">
         <v>700</v>
@@ -1461,7 +1520,7 @@
         <v>6</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
@@ -1488,12 +1547,12 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1">
         <v>800</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>3</v>
       </c>
       <c r="D19" s="1">
@@ -1515,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K19" s="1">
         <v>20</v>
@@ -1542,12 +1601,12 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1">
-        <v>400</v>
-      </c>
-      <c r="C20" s="1">
+        <v>300</v>
+      </c>
+      <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="1">
@@ -1569,279 +1628,734 @@
         <v>2</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1">
+        <v>10</v>
+      </c>
+      <c r="M20" s="1">
+        <v>10</v>
+      </c>
+      <c r="N20" s="1">
+        <v>10</v>
+      </c>
+      <c r="O20" s="1">
+        <v>1</v>
+      </c>
+      <c r="P20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>50</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>5</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="1">
-        <v>10</v>
-      </c>
-      <c r="L20" s="1">
-        <v>10</v>
-      </c>
-      <c r="M20" s="1">
-        <v>10</v>
-      </c>
-      <c r="N20" s="1">
-        <v>10</v>
-      </c>
-      <c r="O20" s="1">
-        <v>1</v>
-      </c>
-      <c r="P20" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>1</v>
-      </c>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="B22" s="1">
+        <v>200</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>80</v>
+      </c>
+      <c r="E22" s="1">
+        <v>40</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1">
+        <v>5</v>
+      </c>
+      <c r="I22" s="1">
+        <v>4</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1">
+        <v>300</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>80</v>
+      </c>
+      <c r="E23" s="1">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
+      <c r="K23" s="1">
+        <v>10</v>
+      </c>
+      <c r="L23" s="1">
+        <v>5</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="1">
+        <v>700</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>100</v>
+      </c>
+      <c r="E24" s="1">
+        <v>60</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>5</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>10</v>
+      </c>
+      <c r="M24" s="1">
+        <v>5</v>
+      </c>
+      <c r="N24" s="1">
+        <v>5</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>2</v>
+      </c>
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>100</v>
+      </c>
+      <c r="E25" s="1">
+        <v>60</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
+        <v>20</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="1">
+        <v>10</v>
+      </c>
+      <c r="L25" s="1">
+        <v>10</v>
+      </c>
+      <c r="M25" s="1">
+        <v>5</v>
+      </c>
+      <c r="N25" s="1">
+        <v>5</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>2</v>
+      </c>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1400</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1">
+        <v>80</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3</v>
+      </c>
+      <c r="J26" s="1">
+        <v>6</v>
+      </c>
+      <c r="K26" s="1">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1">
+        <v>20</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>5</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>3</v>
+      </c>
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1400</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1">
+        <v>80</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="1">
+        <v>10</v>
+      </c>
+      <c r="H27" s="1">
+        <v>10</v>
+      </c>
+      <c r="I27" s="1">
+        <v>3</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>10</v>
+      </c>
+      <c r="M27" s="1">
+        <v>5</v>
+      </c>
+      <c r="N27" s="1">
+        <v>5</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1</v>
+      </c>
+      <c r="P27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>2</v>
+      </c>
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C28" s="1">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>200</v>
+      </c>
+      <c r="E28" s="1">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="1">
+        <v>40</v>
+      </c>
+      <c r="H28" s="1">
+        <v>10</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K28" s="1">
+        <v>20</v>
+      </c>
+      <c r="L28" s="1">
+        <v>10</v>
+      </c>
+      <c r="M28" s="1">
+        <v>10</v>
+      </c>
+      <c r="N28" s="1">
+        <v>10</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1">
+        <v>100</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1">
+        <v>20</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>10</v>
+      </c>
+      <c r="J29" s="1">
+        <v>5</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>10</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>1</v>
+      </c>
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="1">
+        <v>150</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>50</v>
+      </c>
+      <c r="E30" s="1">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>5</v>
+      </c>
+      <c r="M30" s="1">
+        <v>5</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>1</v>
+      </c>
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="1">
+        <v>250</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>50</v>
+      </c>
+      <c r="E31" s="1">
+        <v>50</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>5</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>2</v>
+      </c>
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C32" s="1">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1">
+        <v>500</v>
+      </c>
+      <c r="E32" s="1">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>25</v>
+      </c>
+      <c r="M32" s="1">
+        <v>10</v>
+      </c>
+      <c r="N32" s="1">
+        <v>10</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1">
+        <v>50</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="1">
+        <v>10</v>
+      </c>
+      <c r="H33" s="1">
+        <v>10</v>
+      </c>
+      <c r="I33" s="1">
+        <v>4</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K33" s="1">
+        <v>10</v>
+      </c>
+      <c r="L33" s="1">
+        <v>10</v>
+      </c>
+      <c r="M33" s="1">
+        <v>5</v>
+      </c>
+      <c r="N33" s="1">
+        <v>5</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1</v>
+      </c>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1860,7 +2374,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1879,7 +2393,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1898,7 +2412,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1917,7 +2431,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1936,7 +2450,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1955,7 +2469,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1974,7 +2488,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1993,7 +2507,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2012,7 +2526,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2031,7 +2545,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2050,7 +2564,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2069,7 +2583,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2088,7 +2602,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2107,7 +2621,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>

</xml_diff>

<commit_message>
New troops and new abilities
Added new necromancers and other troops
</commit_message>
<xml_diff>
--- a/documentation/allStats.xlsx
+++ b/documentation/allStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\project_aeii\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF273B8-3CC1-42CE-969F-9179FB21D7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7397B0-51E8-4CCD-AA53-E20B3D18D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20895" yWindow="3555" windowWidth="15345" windowHeight="10035" xr2:uid="{D4135FBB-2C8A-48D4-BC1E-A4B2555D16E4}"/>
+    <workbookView xWindow="14310" yWindow="840" windowWidth="14490" windowHeight="12750" xr2:uid="{D4135FBB-2C8A-48D4-BC1E-A4B2555D16E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
   <si>
     <t>Dataset</t>
   </si>
@@ -253,14 +253,49 @@
   </si>
   <si>
     <t>8, 16, 26, 2, 14</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Skeleton King</t>
+  </si>
+  <si>
+    <t>Mummy Queen</t>
+  </si>
+  <si>
+    <t>Mummy</t>
+  </si>
+  <si>
+    <t>Bat Witch</t>
+  </si>
+  <si>
+    <t>Skeleton Archer</t>
+  </si>
+  <si>
+    <t>29, 9, 11</t>
+  </si>
+  <si>
+    <t>9, 11, 12</t>
+  </si>
+  <si>
+    <t>11, 30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -288,12 +323,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -612,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE6564-BC17-41CE-A57A-346809BD4733}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,13 +1296,13 @@
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M13" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N13" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O13" s="1">
         <v>0</v>
@@ -2282,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M32" s="1">
         <v>10</v>
@@ -2356,121 +2394,331 @@
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1">
+        <v>30</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>2</v>
+      </c>
+      <c r="J34" s="1">
+        <v>11</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>1</v>
+      </c>
       <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>100</v>
+      </c>
+      <c r="E35" s="1">
+        <v>60</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>30</v>
+      </c>
+      <c r="I35" s="1">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>5</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>5</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>2</v>
+      </c>
       <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="1">
+        <v>800</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>300</v>
+      </c>
+      <c r="E36" s="1">
+        <v>10</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>2</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K36" s="1">
+        <v>20</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>1</v>
+      </c>
       <c r="R36" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>150</v>
+      </c>
+      <c r="E37" s="1">
+        <v>30</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>3</v>
+      </c>
+      <c r="J37" s="1">
+        <v>11</v>
+      </c>
+      <c r="K37" s="1">
+        <v>10</v>
+      </c>
+      <c r="L37" s="1">
+        <v>10</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
       <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
+        <v>100</v>
+      </c>
+      <c r="E38" s="1">
+        <v>30</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>10</v>
+      </c>
+      <c r="I38" s="1">
+        <v>3</v>
+      </c>
+      <c r="J38" s="1">
+        <v>31</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>5</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>10</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>4</v>
+      </c>
       <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="1">
+        <v>300</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>50</v>
+      </c>
+      <c r="E39" s="1">
+        <v>60</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
+        <v>5</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>3</v>
+      </c>
       <c r="R39" s="1"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
+      <c r="B40" s="3"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>

</xml_diff>